<commit_message>
Update Cond calibrator to to v0.2.1
Tested & works! Updated example to use sensor on my desk.
cc: @garrigotti, @garrigotti-cws, @shepardb
</commit_message>
<xml_diff>
--- a/utilities/CalibrationProtocolSpreadsheet/Y511-Cond-Calibrator.xlsx
+++ b/utilities/CalibrationProtocolSpreadsheet/Y511-Cond-Calibrator.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaufdenkampe/Documents/Arduino/YosemitechModbus/utilities/CalibrationProtocolSpreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E46CD66-71CF-B745-9572-3951EE8FD621}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FAD503-3EB8-674D-AD65-53EF822D58CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5020" yWindow="-21140" windowWidth="29540" windowHeight="19200" xr2:uid="{A01D2E8A-3A02-234A-9567-63BD2965B45A}"/>
+    <workbookView xWindow="3060" yWindow="-21140" windowWidth="33260" windowHeight="20340" xr2:uid="{A01D2E8A-3A02-234A-9567-63BD2965B45A}"/>
   </bookViews>
   <sheets>
     <sheet name="YL09-example" sheetId="7" r:id="rId1"/>
-    <sheet name="YL09-blank" sheetId="6" r:id="rId2"/>
+    <sheet name="YL09-blank" sheetId="8" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="54">
   <si>
     <t>mS/cm</t>
   </si>
@@ -46,12 +46,6 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>YL0916112101</t>
-  </si>
-  <si>
-    <t>hw 1.2,sw 1.6</t>
-  </si>
-  <si>
     <t>SN:</t>
   </si>
   <si>
@@ -118,9 +112,6 @@
     <t>Calibration Standards: Known Values</t>
   </si>
   <si>
-    <t>Calibration Standards: Measured Values</t>
-  </si>
-  <si>
     <t>Not used in calibration</t>
   </si>
   <si>
@@ -178,21 +169,35 @@
     <t>Rename tab with serial number and date, or keep a workbook for each serial number.</t>
   </si>
   <si>
-    <t>v0.2.0: 2020-09-10</t>
-  </si>
-  <si>
     <t>Type into pale yellow cells G3, J3, M3, P3</t>
+  </si>
+  <si>
+    <t>YL0918031414</t>
+  </si>
+  <si>
+    <t>hw 1.2,sw 1.8</t>
+  </si>
+  <si>
+    <t>v0.2.1: 2020-09-10</t>
+  </si>
+  <si>
+    <t>Calibration Standards: Measured Values (with default K=1 &amp; B=0)</t>
+  </si>
+  <si>
+    <t>Converted units:</t>
+  </si>
+  <si>
+    <t>calibrated X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -329,7 +334,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -339,7 +344,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -355,6 +359,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,14 +527,17 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>136.650125</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>214.29349999999999</c:v>
+                  <c:v>257.74474999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>445.45949999999993</c:v>
+                  <c:v>498.87049999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>903.74919999999997</c:v>
+                  <c:v>986.49012500000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -538,6 +548,9 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>125</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>250</c:v>
                 </c:pt>
@@ -890,14 +903,17 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>136.650125</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>214.29349999999999</c:v>
+                  <c:v>257.74474999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>445.45949999999993</c:v>
+                  <c:v>498.87049999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>903.74919999999997</c:v>
+                  <c:v>986.49012500000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -909,16 +925,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-0.60071942311057569</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.62686231229534428</c:v>
+                  <c:v>-0.27799536020171445</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.94305805765918649</c:v>
+                  <c:v>1.4624169967622151</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.31619574536375694</c:v>
+                  <c:v>-0.58370221344989659</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1334,7 +1350,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-AB3C-9F48-8884-38C25ACB1FCC}"/>
+              <c16:uniqueId val="{00000001-A258-3C48-9173-A32C63CCFB96}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1710,7 +1726,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5405-054A-8E2C-709CACC4D456}"/>
+              <c16:uniqueId val="{00000001-8CFF-2F42-9791-61536E450AD9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1936,16 +1952,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>105833</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>118533</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>48684</xdr:rowOff>
+      <xdr:rowOff>16934</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1974,16 +1990,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>105834</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>63501</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>105834</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>332317</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>175684</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2017,23 +2033,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>105833</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>118533</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>48684</xdr:rowOff>
+      <xdr:rowOff>16934</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8391F21-CF98-3241-9C43-ED5FE6A01DD0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{368BDB3E-4288-AE44-8FC5-794901C9622B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2055,23 +2071,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>105834</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>63501</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>105834</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>332317</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>175684</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C12DE84E-5FE6-C247-A95C-EBD30B8CFF19}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44A31521-FBAA-7A47-86C5-D35E1DC6A71D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2391,10 +2407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8398C2D1-1195-E443-A486-6715ED3C5E41}">
-  <dimension ref="A1:T54"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2415,37 +2431,37 @@
   <sheetData>
     <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
+      <c r="H2" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
     </row>
     <row r="3" spans="1:18" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>23</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>4</v>
@@ -2481,393 +2497,361 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="E4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
     </row>
     <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="A5" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
       <c r="E5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24" t="s">
+      <c r="I5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="L5" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24" t="s">
+      <c r="L5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24" t="s">
+      <c r="O5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="R5" s="24" t="s">
-        <v>13</v>
+      <c r="R5" s="23" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="13">
-        <v>43368</v>
-      </c>
-      <c r="E6" s="7">
-        <v>-1.4416999999999999E-2</v>
-      </c>
-      <c r="F6" s="7">
-        <v>22.311520000000002</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+        <v>44084</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="H6" s="7">
+        <v>0.13739699999999999</v>
+      </c>
+      <c r="I6" s="7">
+        <v>23.147490000000001</v>
+      </c>
       <c r="K6" s="7">
-        <v>0.21482399999999999</v>
+        <v>0.25834499999999999</v>
       </c>
       <c r="L6" s="7">
-        <v>22.35867</v>
+        <v>23.321750000000002</v>
       </c>
       <c r="N6" s="7">
-        <v>0.44702999999999998</v>
+        <v>0.498859</v>
       </c>
       <c r="O6" s="7">
-        <v>22.359919999999999</v>
+        <v>22.73395</v>
       </c>
       <c r="Q6" s="7">
-        <v>0.904138</v>
+        <v>0.98693699999999995</v>
       </c>
       <c r="R6" s="7">
-        <v>22.33136</v>
+        <v>22.751860000000001</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="E7" s="7">
-        <v>-1.5023E-2</v>
-      </c>
-      <c r="F7" s="7">
-        <v>22.252040000000001</v>
-      </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="H7" s="7">
+        <v>0.136182</v>
+      </c>
+      <c r="I7" s="7">
+        <v>23.161799999999999</v>
+      </c>
       <c r="K7" s="7">
-        <v>0.21498700000000001</v>
+        <v>0.25811400000000001</v>
       </c>
       <c r="L7" s="7">
-        <v>22.420839999999998</v>
+        <v>23.328309999999998</v>
       </c>
       <c r="N7" s="7">
-        <v>0.444996</v>
+        <v>0.499751</v>
       </c>
       <c r="O7" s="7">
-        <v>22.382259999999999</v>
+        <v>22.736509999999999</v>
       </c>
       <c r="Q7" s="7">
-        <v>0.90412300000000001</v>
+        <v>0.98677499999999996</v>
       </c>
       <c r="R7" s="7">
-        <v>22.340060000000001</v>
+        <v>22.754390000000001</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="7">
-        <v>-1.4959999999999999E-2</v>
-      </c>
-      <c r="F8" s="7">
-        <v>22.315249999999999</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="H8" s="7">
+        <v>0.136934</v>
+      </c>
+      <c r="I8" s="7">
+        <v>23.17474</v>
+      </c>
       <c r="K8" s="7">
-        <v>0.21466499999999999</v>
+        <v>0.25824399999999997</v>
       </c>
       <c r="L8" s="7">
-        <v>22.419560000000001</v>
+        <v>23.332180000000001</v>
       </c>
       <c r="N8" s="7">
-        <v>0.44487199999999999</v>
+        <v>0.499751</v>
       </c>
       <c r="O8" s="7">
-        <v>22.38477</v>
+        <v>22.737729999999999</v>
       </c>
       <c r="Q8" s="7">
-        <v>0.90381500000000004</v>
+        <v>0.98677499999999996</v>
       </c>
       <c r="R8" s="7">
-        <v>22.28302</v>
+        <v>22.756959999999999</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="7">
-        <v>-1.4959999999999999E-2</v>
-      </c>
-      <c r="F9" s="7">
-        <v>22.31644</v>
-      </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+        <v>48</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="H9" s="7">
+        <v>0.136934</v>
+      </c>
+      <c r="I9" s="7">
+        <v>23.185120000000001</v>
+      </c>
       <c r="K9" s="7">
-        <v>0.21507499999999999</v>
+        <v>0.25824399999999997</v>
       </c>
       <c r="L9" s="7">
-        <v>22.420839999999998</v>
+        <v>23.337399999999999</v>
       </c>
       <c r="N9" s="7">
-        <v>0.44620799999999999</v>
+        <v>0.49938900000000003</v>
       </c>
       <c r="O9" s="7">
-        <v>22.367339999999999</v>
+        <v>22.74033</v>
       </c>
       <c r="Q9" s="7">
-        <v>0.90431700000000004</v>
+        <v>0.98643499999999995</v>
       </c>
       <c r="R9" s="7">
-        <v>22.351199999999999</v>
+        <v>22.756959999999999</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="7">
-        <v>-1.5127E-2</v>
-      </c>
-      <c r="F10" s="7">
-        <v>22.318940000000001</v>
-      </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+        <v>49</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="H10" s="7">
+        <v>0.136214</v>
+      </c>
+      <c r="I10" s="7">
+        <v>23.194210000000002</v>
+      </c>
       <c r="K10" s="7">
-        <v>0.21507499999999999</v>
+        <v>0.25700899999999999</v>
       </c>
       <c r="L10" s="7">
-        <v>22.422029999999999</v>
+        <v>23.341339999999999</v>
       </c>
       <c r="N10" s="7">
-        <v>0.44517000000000001</v>
+        <v>0.496529</v>
       </c>
       <c r="O10" s="7">
-        <v>22.390989999999999</v>
+        <v>22.745450000000002</v>
       </c>
       <c r="Q10" s="7">
-        <v>0.90306200000000003</v>
+        <v>0.98643499999999995</v>
       </c>
       <c r="R10" s="7">
-        <v>22.35492</v>
+        <v>22.758240000000001</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="7">
-        <v>-1.5330999999999999E-2</v>
-      </c>
-      <c r="F11" s="7">
-        <v>22.318940000000001</v>
-      </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+        <v>22</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="H11" s="7">
+        <v>0.136214</v>
+      </c>
+      <c r="I11" s="7">
+        <v>23.204619999999998</v>
+      </c>
       <c r="K11" s="7">
-        <v>0.21477299999999999</v>
+        <v>0.25743100000000002</v>
       </c>
       <c r="L11" s="7">
-        <v>22.420839999999998</v>
+        <v>23.34393</v>
       </c>
       <c r="N11" s="7">
-        <v>0.44566499999999998</v>
+        <v>0.49766899999999997</v>
       </c>
       <c r="O11" s="7">
-        <v>22.371089999999999</v>
+        <v>22.746729999999999</v>
       </c>
       <c r="Q11" s="7">
-        <v>0.90357500000000002</v>
+        <v>0.98612299999999997</v>
       </c>
       <c r="R11" s="7">
-        <v>22.325130000000001</v>
+        <v>22.762119999999999</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" s="14">
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="7">
-        <v>-1.5018E-2</v>
-      </c>
-      <c r="F12" s="7">
-        <v>22.32263</v>
-      </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="H12" s="7">
+        <v>0.13667199999999999</v>
+      </c>
+      <c r="I12" s="7">
+        <v>23.213709999999999</v>
+      </c>
       <c r="K12" s="7">
-        <v>0.21337300000000001</v>
+        <v>0.25743100000000002</v>
       </c>
       <c r="L12" s="7">
-        <v>22.422029999999999</v>
+        <v>23.346530000000001</v>
       </c>
       <c r="N12" s="7">
-        <v>0.445185</v>
+        <v>0.49971599999999999</v>
       </c>
       <c r="O12" s="7">
-        <v>22.39218</v>
+        <v>22.74802</v>
       </c>
       <c r="Q12" s="7">
-        <v>0.90297300000000003</v>
+        <v>0.98612299999999997</v>
       </c>
       <c r="R12" s="7">
-        <v>22.363620000000001</v>
+        <v>22.763400000000001</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="14">
-        <v>1.9400000000000001E-2</v>
+        <v>-2.0999999999999999E-3</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="7">
-        <v>-1.5018E-2</v>
-      </c>
-      <c r="F13" s="7">
-        <v>22.315249999999999</v>
-      </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="H13" s="7">
+        <v>0.136654</v>
+      </c>
+      <c r="I13" s="7">
+        <v>23.221499999999999</v>
+      </c>
       <c r="K13" s="7">
-        <v>0.21321999999999999</v>
+        <v>0.25713999999999998</v>
       </c>
       <c r="L13" s="7">
-        <v>22.420839999999998</v>
+        <v>23.34787</v>
       </c>
       <c r="N13" s="7">
-        <v>0.44518000000000002</v>
+        <v>0.49930000000000002</v>
       </c>
       <c r="O13" s="7">
-        <v>22.39594</v>
+        <v>22.750579999999999</v>
       </c>
       <c r="Q13" s="7">
-        <v>0.90343700000000005</v>
+        <v>0.98631800000000003</v>
       </c>
       <c r="R13" s="7">
-        <v>22.363620000000001</v>
+        <v>22.76465</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="E14" s="7">
-        <v>-1.546E-2</v>
-      </c>
-      <c r="F14" s="7">
-        <v>22.315249999999999</v>
-      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
-      <c r="K14" s="7">
-        <v>0.21315000000000001</v>
-      </c>
-      <c r="L14" s="7">
-        <v>22.423310000000001</v>
-      </c>
-      <c r="N14" s="7">
-        <v>0.44518999999999997</v>
-      </c>
-      <c r="O14" s="7">
-        <v>22.374790000000001</v>
-      </c>
-      <c r="Q14" s="7">
-        <v>0.90417700000000001</v>
-      </c>
-      <c r="R14" s="7">
-        <v>22.305299999999999</v>
-      </c>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
     </row>
     <row r="15" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="7">
-        <v>-1.5128000000000001E-2</v>
-      </c>
-      <c r="F15" s="7">
-        <v>22.325130000000001</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
-      <c r="K15" s="7">
-        <v>0.21379300000000001</v>
-      </c>
-      <c r="L15" s="7">
-        <v>22.361149999999999</v>
-      </c>
-      <c r="N15" s="7">
-        <v>0.44509900000000002</v>
-      </c>
-      <c r="O15" s="7">
-        <v>22.39716</v>
-      </c>
-      <c r="Q15" s="7">
-        <v>0.90387499999999998</v>
-      </c>
-      <c r="R15" s="7">
-        <v>22.368590000000001</v>
-      </c>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" s="15">
         <v>1</v>
@@ -2875,9 +2859,9 @@
       <c r="E16" s="15"/>
       <c r="F16" s="16"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A17" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17" s="15">
         <v>0</v>
@@ -2886,695 +2870,460 @@
       <c r="D17" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="9" t="e">
         <f>AVERAGE(E6:E15)</f>
-        <v>-1.5044199999999999E-2</v>
-      </c>
-      <c r="F17" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F17" s="10" t="e">
         <f>AVERAGE(F6:F15)</f>
-        <v>22.311139000000001</v>
-      </c>
-      <c r="H17" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="9">
         <f>AVERAGE(H6:H15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I17" s="10" t="e">
+        <v>0.13665012500000001</v>
+      </c>
+      <c r="I17" s="10">
         <f>AVERAGE(I6:I15)</f>
-        <v>#DIV/0!</v>
+        <v>23.187898749999999</v>
       </c>
       <c r="K17" s="9">
         <f>AVERAGE(K6:K15)</f>
-        <v>0.2142935</v>
+        <v>0.25774474999999997</v>
       </c>
       <c r="L17" s="10">
         <f>AVERAGE(L6:L15)</f>
-        <v>22.409011000000003</v>
+        <v>23.33741375</v>
       </c>
       <c r="N17" s="9">
         <f>AVERAGE(N6:N15)</f>
-        <v>0.44545949999999995</v>
+        <v>0.49887049999999999</v>
       </c>
       <c r="O17" s="10">
         <f>AVERAGE(O6:O15)</f>
-        <v>22.381644000000001</v>
+        <v>22.7424125</v>
       </c>
       <c r="Q17" s="9">
         <f>AVERAGE(Q6:Q15)</f>
-        <v>0.90374920000000003</v>
+        <v>0.986490125</v>
       </c>
       <c r="R17" s="10">
         <f>AVERAGE(R6:R15)</f>
-        <v>22.338681999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+        <v>22.7585725</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
       <c r="C18" s="12"/>
       <c r="D18" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="9" t="e">
         <f>STDEV(E6:E15)</f>
-        <v>2.745508655564171E-4</v>
-      </c>
-      <c r="F18" s="10">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F18" s="10" t="e">
         <f>STDEV(F6:F15)</f>
-        <v>2.1137488787039416E-2</v>
-      </c>
-      <c r="H18" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H18" s="9">
         <f>STDEV(H6:H15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" s="10" t="e">
+        <v>4.3408966733350413E-4</v>
+      </c>
+      <c r="I18" s="10">
         <f>STDEV(I6:I15)</f>
-        <v>#DIV/0!</v>
+        <v>2.5661485001845986E-2</v>
       </c>
       <c r="K18" s="9">
         <f>STDEV(K6:K15)</f>
-        <v>8.1032260379568244E-4</v>
+        <v>5.4760198006528705E-4</v>
       </c>
       <c r="L18" s="10">
         <f>STDEV(L6:L15)</f>
-        <v>2.5904362759967638E-2</v>
+        <v>9.3039145947130236E-3</v>
       </c>
       <c r="N18" s="9">
         <f>STDEV(N6:N15)</f>
-        <v>6.7237658925468902E-4</v>
+        <v>1.1738276826568049E-3</v>
       </c>
       <c r="O18" s="10">
         <f>STDEV(O6:O15)</f>
-        <v>1.2860486598708443E-2</v>
+        <v>6.0796540080127167E-3</v>
       </c>
       <c r="Q18" s="9">
         <f>STDEV(Q6:Q15)</f>
-        <v>4.7363858701662419E-4</v>
+        <v>3.0874651530710264E-4</v>
       </c>
       <c r="R18" s="10">
         <f>STDEV(R6:R15)</f>
-        <v>2.7909481781884519E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+        <v>4.4831008082733288E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="11" t="e">
         <f>E18/E17</f>
-        <v>-1.8249615503411091E-2</v>
-      </c>
-      <c r="F19" s="11">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F19" s="11" t="e">
         <f>F18/F17</f>
-        <v>9.4739622154832231E-4</v>
-      </c>
-      <c r="H19" s="11" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" s="11">
         <f>H18/H17</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I19" s="11" t="e">
+        <v>3.1766503494490336E-3</v>
+      </c>
+      <c r="I19" s="11">
         <f>I18/I17</f>
-        <v>#DIV/0!</v>
+        <v>1.1066757397259202E-3</v>
       </c>
       <c r="K19" s="11">
         <f>K18/K17</f>
-        <v>3.7813680946724116E-3</v>
+        <v>2.1245902392397404E-3</v>
       </c>
       <c r="L19" s="11">
         <f>L18/L17</f>
-        <v>1.1559797422549185E-3</v>
+        <v>3.9866947959102899E-4</v>
       </c>
       <c r="N19" s="11">
         <f>N18/N17</f>
-        <v>1.5094000447957426E-3</v>
+        <v>2.3529707261840597E-3</v>
       </c>
       <c r="O19" s="11">
         <f>O18/O17</f>
-        <v>5.7459972997106208E-4</v>
+        <v>2.6732669667357042E-4</v>
       </c>
       <c r="Q19" s="11">
         <f>Q18/Q17</f>
-        <v>5.2408188800236188E-4</v>
+        <v>3.1297476526397327E-4</v>
       </c>
       <c r="R19" s="11">
         <f>R18/R17</f>
-        <v>1.2493790717771317E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+        <v>1.9698514958586829E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="8">
+        <v>52</v>
+      </c>
+      <c r="E20" s="8" t="e">
         <f>E17*1000</f>
-        <v>-15.044199999999998</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="8" t="e">
+      <c r="H20" s="8">
         <f>H17*1000</f>
-        <v>#DIV/0!</v>
+        <v>136.650125</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>4</v>
       </c>
       <c r="K20" s="8">
         <f>K17*1000</f>
-        <v>214.29349999999999</v>
+        <v>257.74474999999995</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>4</v>
       </c>
       <c r="N20" s="8">
         <f>N17*1000</f>
-        <v>445.45949999999993</v>
+        <v>498.87049999999999</v>
       </c>
       <c r="O20" s="3" t="s">
         <v>4</v>
       </c>
       <c r="Q20" s="8">
         <f>Q17*1000</f>
-        <v>903.74919999999997</v>
+        <v>986.49012500000003</v>
       </c>
       <c r="R20" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="S23" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="T23" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+        <v>30</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="T23" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="U23" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="23" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="S24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="T24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T24" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="U24" s="23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="H25" s="8" t="str">
-        <f>IF(ISNUMBER(E25), FORECAST(E25,$F$25:$F$28,$E$25:$E$28), "")</f>
-        <v/>
-      </c>
-      <c r="I25" s="8" t="str">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="E25" s="24">
+        <f t="shared" ref="E25:F28" si="0">T25</f>
+        <v>136.650125</v>
+      </c>
+      <c r="F25" s="24">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="H25" s="8">
+        <f t="shared" ref="H25" si="1">IF(ISNUMBER(E25), FORECAST(E25,$F$25:$F$28,$E$25:$E$28), "")</f>
+        <v>125.60071942311058</v>
+      </c>
+      <c r="I25" s="8">
         <f>IF(ISNUMBER(F25), F25-H25, "")</f>
-        <v/>
-      </c>
-      <c r="S25" s="8" t="e">
+        <v>-0.60071942311057569</v>
+      </c>
+      <c r="K25" s="8">
+        <f>(E25+$F$32) * $F$31</f>
+        <v>125.15420619887915</v>
+      </c>
+      <c r="T25" s="8">
         <f>H20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T25" s="8">
+        <v>136.650125</v>
+      </c>
+      <c r="U25" s="8">
         <f>H3</f>
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="25">
-        <f t="shared" ref="E26:F28" si="0">S26</f>
-        <v>214.29349999999999</v>
-      </c>
-      <c r="F26" s="25">
+        <v>42</v>
+      </c>
+      <c r="E26" s="24">
+        <f t="shared" si="0"/>
+        <v>257.74474999999995</v>
+      </c>
+      <c r="F26" s="24">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
       <c r="H26" s="8">
-        <f t="shared" ref="H26:H28" si="1">IF(ISNUMBER(E26), FORECAST(E26,$F$25:$F$28,$E$25:$E$28), "")</f>
-        <v>249.37313768770466</v>
+        <f t="shared" ref="H26:H28" si="2">IF(ISNUMBER(E26), FORECAST(E26,$F$25:$F$28,$E$25:$E$28), "")</f>
+        <v>250.27799536020171</v>
       </c>
       <c r="I26" s="8">
         <f>IF(ISNUMBER(F26), F26-H26, "")</f>
-        <v>0.62686231229534428</v>
-      </c>
-      <c r="S26" s="8">
+        <v>-0.27799536020171445</v>
+      </c>
+      <c r="K26" s="8">
+        <f t="shared" ref="K26:K28" si="3">(E26+$F$32) * $F$31</f>
+        <v>249.83148213597033</v>
+      </c>
+      <c r="T26" s="8">
         <f>K20</f>
-        <v>214.29349999999999</v>
-      </c>
-      <c r="T26" s="8">
+        <v>257.74474999999995</v>
+      </c>
+      <c r="U26" s="8">
         <f>K3</f>
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="25">
+        <v>43</v>
+      </c>
+      <c r="E27" s="24">
         <f t="shared" si="0"/>
-        <v>445.45949999999993</v>
-      </c>
-      <c r="F27" s="25">
+        <v>498.87049999999999</v>
+      </c>
+      <c r="F27" s="24">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="H27" s="8">
-        <f t="shared" si="1"/>
-        <v>500.94305805765919</v>
+        <f t="shared" si="2"/>
+        <v>498.53758300323778</v>
       </c>
       <c r="I27" s="8">
-        <f t="shared" ref="I27:I28" si="2">IF(ISNUMBER(F27), F27-H27, "")</f>
-        <v>-0.94305805765918649</v>
-      </c>
-      <c r="S27" s="8">
+        <f t="shared" ref="I27:I28" si="4">IF(ISNUMBER(F27), F27-H27, "")</f>
+        <v>1.4624169967622151</v>
+      </c>
+      <c r="K27" s="8">
+        <f t="shared" si="3"/>
+        <v>498.09106977900632</v>
+      </c>
+      <c r="T27" s="8">
         <f>N20</f>
-        <v>445.45949999999993</v>
-      </c>
-      <c r="T27" s="8">
+        <v>498.87049999999999</v>
+      </c>
+      <c r="U27" s="8">
         <f>N3</f>
         <v>500</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E28" s="25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="E28" s="24">
         <f t="shared" si="0"/>
-        <v>903.74919999999997</v>
-      </c>
-      <c r="F28" s="25">
+        <v>986.49012500000003</v>
+      </c>
+      <c r="F28" s="24">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="H28" s="8">
-        <f t="shared" si="1"/>
-        <v>999.68380425463624</v>
+        <f t="shared" si="2"/>
+        <v>1000.5837022134499</v>
       </c>
       <c r="I28" s="8">
-        <f t="shared" si="2"/>
-        <v>0.31619574536375694</v>
-      </c>
-      <c r="S28" s="8">
+        <f t="shared" si="4"/>
+        <v>-0.58370221344989659</v>
+      </c>
+      <c r="K28" s="8">
+        <f t="shared" si="3"/>
+        <v>1000.1371889892185</v>
+      </c>
+      <c r="T28" s="8">
         <f>Q20</f>
-        <v>903.74919999999997</v>
-      </c>
-      <c r="T28" s="8">
+        <v>986.49012500000003</v>
+      </c>
+      <c r="U28" s="8">
         <f>Q3</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="S30" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+        <v>45</v>
+      </c>
+      <c r="T30" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A31" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="27">
+        <v>8</v>
+      </c>
+      <c r="B31" s="26">
         <f>F31</f>
-        <v>1.0882652309161149</v>
+        <v>1.02958554879782</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F31" s="9">
         <f>SLOPE($F$25:$F$28,$E$25:$E$28)</f>
-        <v>1.0882652309161149</v>
-      </c>
-      <c r="S31" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
+        <v>1.02958554879782</v>
+      </c>
+      <c r="T31" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A32" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="27">
+        <v>9</v>
+      </c>
+      <c r="B32" s="26">
         <f>F34</f>
-        <v>1.6164972426382179E-2</v>
+        <v>-1.5092274518305146E-2</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F32" s="9">
         <f>INTERCEPT($F$25:$F$28,$E$25:$E$28)</f>
-        <v>16.164972426382178</v>
+        <v>-15.092274518305146</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="S32" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="F33" s="26"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="T32" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F33" s="25"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="18"/>
       <c r="E34" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F34" s="9">
         <f>F32/1000</f>
-        <v>1.6164972426382179E-2</v>
+        <v>-1.5092274518305146E-2</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="E37" s="12"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="E38" s="12"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="H44" s="8">
-        <f>H46*1000</f>
-        <v>947.51800000000003</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K44" s="8">
-        <f>K46*1000</f>
-        <v>512.36275000000001</v>
-      </c>
-      <c r="L44" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="N44" s="8">
-        <f>N46*1000</f>
-        <v>218.41399999999999</v>
-      </c>
-      <c r="O44" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q44" s="8">
-        <f>Q46*1000</f>
-        <v>-0.3745</v>
-      </c>
-      <c r="R44" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="H45" s="19">
-        <f>H42/H44</f>
-        <v>0</v>
-      </c>
-      <c r="K45" s="19">
-        <f>K42/K44</f>
-        <v>0</v>
-      </c>
-      <c r="N45" s="19">
-        <f>N42/N44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="H46" s="9">
-        <f>AVERAGE(H51:H60)</f>
-        <v>0.94751800000000008</v>
-      </c>
-      <c r="I46" s="10">
-        <f>AVERAGE(I51:I60)</f>
-        <v>22.315552500000003</v>
-      </c>
-      <c r="K46" s="9">
-        <f>AVERAGE(K51:K60)</f>
-        <v>0.51236274999999998</v>
-      </c>
-      <c r="L46" s="10">
-        <f>AVERAGE(L51:L60)</f>
-        <v>22.345009999999998</v>
-      </c>
-      <c r="N46" s="9">
-        <f>AVERAGE(N51:N60)</f>
-        <v>0.218414</v>
-      </c>
-      <c r="O46" s="10">
-        <f>AVERAGE(O51:O60)</f>
-        <v>22.387239999999998</v>
-      </c>
-      <c r="Q46" s="9">
-        <f>AVERAGE(Q51:Q60)</f>
-        <v>-3.745E-4</v>
-      </c>
-      <c r="R46" s="10">
-        <f>AVERAGE(R51:R60)</f>
-        <v>22.335697499999998</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="H47" s="9">
-        <f>STDEV(H51:H60)</f>
-        <v>3.4982567087048835E-4</v>
-      </c>
-      <c r="I47" s="10">
-        <f>STDEV(I51:I60)</f>
-        <v>3.1823759860624558E-2</v>
-      </c>
-      <c r="K47" s="9">
-        <f>STDEV(K51:K60)</f>
-        <v>4.0161704396105946E-4</v>
-      </c>
-      <c r="L47" s="10">
-        <f>STDEV(L51:L60)</f>
-        <v>2.3824492999153329E-2</v>
-      </c>
-      <c r="N47" s="9">
-        <f>STDEV(N51:N60)</f>
-        <v>6.4849106907240769E-4</v>
-      </c>
-      <c r="O47" s="10">
-        <f>STDEV(O51:O60)</f>
-        <v>3.0061910562481638E-2</v>
-      </c>
-      <c r="Q47" s="9">
-        <f>STDEV(Q51:Q60)</f>
-        <v>8.0289061106313453E-5</v>
-      </c>
-      <c r="R47" s="10">
-        <f>STDEV(R51:R60)</f>
-        <v>3.0177420228817243E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="H48" s="11">
-        <f>H47/H46</f>
-        <v>3.6920213744803614E-4</v>
-      </c>
-      <c r="I48" s="11">
-        <f>I47/I46</f>
-        <v>1.4260798544254978E-3</v>
-      </c>
-      <c r="K48" s="11">
-        <f>K47/K46</f>
-        <v>7.8385293224587363E-4</v>
-      </c>
-      <c r="L48" s="11">
-        <f>L47/L46</f>
-        <v>1.0662108899997507E-3</v>
-      </c>
-      <c r="N48" s="11">
-        <f>N47/N46</f>
-        <v>2.9690911254425436E-3</v>
-      </c>
-      <c r="O48" s="11">
-        <f>O47/O46</f>
-        <v>1.3428145033725302E-3</v>
-      </c>
-      <c r="Q48" s="11">
-        <f>Q47/Q46</f>
-        <v>-0.21439001630524288</v>
-      </c>
-      <c r="R48" s="11">
-        <f>R47/R46</f>
-        <v>1.3510847480280052E-3</v>
-      </c>
-    </row>
-    <row r="49" spans="8:18" x14ac:dyDescent="0.15">
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="K49" s="11"/>
-      <c r="L49" s="11"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-    </row>
-    <row r="51" spans="8:18" x14ac:dyDescent="0.15">
-      <c r="H51" s="7">
-        <v>0.94756799999999997</v>
-      </c>
-      <c r="I51" s="7">
-        <v>22.326419999999999</v>
-      </c>
-      <c r="K51" s="7">
-        <v>0.51254699999999997</v>
-      </c>
-      <c r="L51" s="7">
-        <v>22.310269999999999</v>
-      </c>
-      <c r="N51" s="7">
-        <v>0.21909000000000001</v>
-      </c>
-      <c r="O51" s="7">
-        <v>22.408359999999998</v>
-      </c>
-      <c r="Q51" s="7">
-        <v>-3.59E-4</v>
-      </c>
-      <c r="R51" s="7">
-        <v>22.351199999999999</v>
-      </c>
-    </row>
-    <row r="52" spans="8:18" x14ac:dyDescent="0.15">
-      <c r="H52" s="7">
-        <v>0.94742999999999999</v>
-      </c>
-      <c r="I52" s="7">
-        <v>22.268129999999999</v>
-      </c>
-      <c r="K52" s="7">
-        <v>0.51281100000000002</v>
-      </c>
-      <c r="L52" s="7">
-        <v>22.34995</v>
-      </c>
-      <c r="N52" s="7">
-        <v>0.217916</v>
-      </c>
-      <c r="O52" s="7">
-        <v>22.34995</v>
-      </c>
-      <c r="Q52" s="7">
-        <v>-4.17E-4</v>
-      </c>
-      <c r="R52" s="7">
-        <v>22.34995</v>
-      </c>
-    </row>
-    <row r="53" spans="8:18" x14ac:dyDescent="0.15">
-      <c r="H53" s="7">
-        <v>0.947959</v>
-      </c>
-      <c r="I53" s="7">
-        <v>22.33258</v>
-      </c>
-      <c r="K53" s="7">
-        <v>0.51188999999999996</v>
-      </c>
-      <c r="L53" s="7">
-        <v>22.356200000000001</v>
-      </c>
-      <c r="N53" s="7">
-        <v>0.217805</v>
-      </c>
-      <c r="O53" s="7">
-        <v>22.41461</v>
-      </c>
-      <c r="Q53" s="7">
-        <v>-4.5300000000000001E-4</v>
-      </c>
-      <c r="R53" s="7">
-        <v>22.351199999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="8:18" x14ac:dyDescent="0.15">
-      <c r="H54" s="7">
-        <v>0.94711500000000004</v>
-      </c>
-      <c r="I54" s="7">
-        <v>22.335080000000001</v>
-      </c>
-      <c r="K54" s="7">
-        <v>0.51220299999999996</v>
-      </c>
-      <c r="L54" s="7">
-        <v>22.363620000000001</v>
-      </c>
-      <c r="N54" s="7">
-        <v>0.21884500000000001</v>
-      </c>
-      <c r="O54" s="7">
-        <v>22.37604</v>
-      </c>
-      <c r="Q54" s="7">
-        <v>-2.6899999999999998E-4</v>
-      </c>
-      <c r="R54" s="7">
-        <v>22.29044</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3583,11 +3332,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A79A962D-6FE3-4441-B9CE-70AD44481102}">
-  <dimension ref="A1:T54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{001CAD04-9A93-294E-A9C1-B00706AE1E91}">
+  <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B13"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3608,36 +3357,36 @@
   <sheetData>
     <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
+      <c r="H2" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
     </row>
     <row r="3" spans="1:18" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="20"/>
+        <v>17</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="19"/>
       <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
@@ -3664,65 +3413,65 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="E4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
     </row>
     <row r="5" spans="1:18" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="A5" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
       <c r="E5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24" t="s">
+      <c r="I5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="L5" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24" t="s">
+      <c r="L5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24" t="s">
+      <c r="O5" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="R5" s="24" t="s">
-        <v>13</v>
+      <c r="R5" s="23" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="13"/>
       <c r="E6" s="7"/>
@@ -3750,7 +3499,7 @@
     </row>
     <row r="8" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -3765,7 +3514,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="7"/>
       <c r="E9" s="7"/>
@@ -3781,7 +3530,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="7"/>
       <c r="E10" s="7"/>
@@ -3797,10 +3546,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -3815,11 +3564,11 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -3834,11 +3583,11 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -3865,7 +3614,7 @@
     </row>
     <row r="15" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -3880,7 +3629,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" s="15">
         <v>1</v>
@@ -3888,9 +3637,9 @@
       <c r="E16" s="15"/>
       <c r="F16" s="16"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A17" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17" s="15">
         <v>0</v>
@@ -3940,7 +3689,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
       <c r="C18" s="12"/>
       <c r="D18" s="12" t="s">
         <v>2</v>
@@ -3986,9 +3735,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="12" t="s">
@@ -4035,13 +3784,13 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="E20" s="8" t="e">
         <f>E17*1000</f>
@@ -4079,218 +3828,237 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+        <v>40</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="S23" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="T23" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+        <v>30</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="T23" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="U23" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="23" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="S24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="T24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T24" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="U24" s="23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E25" s="25" t="e">
-        <f t="shared" ref="E25" si="0">S25</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F25" s="25">
-        <f t="shared" ref="F25" si="1">T25</f>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="E25" s="24" t="e">
+        <f t="shared" ref="E25:F28" si="0">T25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F25" s="24">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H25" s="8" t="str">
-        <f>IF(ISNUMBER(E25), FORECAST(E25,$F$25:$F$28,$E$25:$E$28), "")</f>
+        <f t="shared" ref="H25:H28" si="1">IF(ISNUMBER(E25), FORECAST(E25,$F$25:$F$28,$E$25:$E$28), "")</f>
         <v/>
       </c>
       <c r="I25" s="8" t="e">
         <f>IF(ISNUMBER(F25), F25-H25, "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="S25" s="8" t="e">
+      <c r="K25" s="8" t="e">
+        <f>(E25+$F$32) * $F$31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T25" s="8" t="e">
         <f>H20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T25" s="8">
+      <c r="U25" s="8">
         <f>H3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="25" t="e">
-        <f t="shared" ref="E26:F28" si="2">S26</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F26" s="25">
-        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="E26" s="24" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F26" s="24">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H26" s="8" t="str">
-        <f t="shared" ref="H26:H28" si="3">IF(ISNUMBER(E26), FORECAST(E26,$F$25:$F$28,$E$25:$E$28), "")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I26" s="8" t="e">
         <f>IF(ISNUMBER(F26), F26-H26, "")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="S26" s="8" t="e">
+      <c r="K26" s="8" t="e">
+        <f t="shared" ref="K26:K28" si="2">(E26+$F$32) * $F$31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T26" s="8" t="e">
         <f>K20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T26" s="8">
+      <c r="U26" s="8">
         <f>K3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="25" t="e">
+        <v>43</v>
+      </c>
+      <c r="E27" s="24" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F27" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I27" s="8" t="e">
+        <f t="shared" ref="I27:I28" si="3">IF(ISNUMBER(F27), F27-H27, "")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K27" s="8" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F27" s="25">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H27" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I27" s="8" t="e">
-        <f t="shared" ref="I27:I28" si="4">IF(ISNUMBER(F27), F27-H27, "")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S27" s="8" t="e">
+      <c r="T27" s="8" t="e">
         <f>N20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T27" s="8">
+      <c r="U27" s="8">
         <f>N3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E28" s="25" t="e">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="E28" s="24" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F28" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I28" s="8" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K28" s="8" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F28" s="25">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H28" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I28" s="8" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S28" s="8" t="e">
+      <c r="T28" s="8" t="e">
         <f>Q20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="T28" s="8">
+      <c r="U28" s="8">
         <f>Q3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="S30" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+        <v>45</v>
+      </c>
+      <c r="T30" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A31" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="27" t="e">
+        <v>8</v>
+      </c>
+      <c r="B31" s="26" t="e">
         <f>F31</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F31" s="9" t="e">
         <f>SLOPE($F$25:$F$28,$E$25:$E$28)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S31" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
+      <c r="T31" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A32" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="27" t="e">
+        <v>9</v>
+      </c>
+      <c r="B32" s="26" t="e">
         <f>F34</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F32" s="9" t="e">
         <f>INTERCEPT($F$25:$F$28,$E$25:$E$28)</f>
@@ -4299,17 +4067,17 @@
       <c r="G32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="S32" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="F33" s="26"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="T32" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="F33" s="25"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="18"/>
       <c r="E34" s="12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F34" s="9" t="e">
         <f>F32/1000</f>
@@ -4319,281 +4087,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="E37" s="12"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="E38" s="12"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="H44" s="8">
-        <f>H46*1000</f>
-        <v>947.51800000000003</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K44" s="8">
-        <f>K46*1000</f>
-        <v>512.36275000000001</v>
-      </c>
-      <c r="L44" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="N44" s="8">
-        <f>N46*1000</f>
-        <v>218.41399999999999</v>
-      </c>
-      <c r="O44" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q44" s="8">
-        <f>Q46*1000</f>
-        <v>-0.3745</v>
-      </c>
-      <c r="R44" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="H45" s="19">
-        <f>H42/H44</f>
-        <v>0</v>
-      </c>
-      <c r="K45" s="19">
-        <f>K42/K44</f>
-        <v>0</v>
-      </c>
-      <c r="N45" s="19">
-        <f>N42/N44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="H46" s="9">
-        <f>AVERAGE(H51:H60)</f>
-        <v>0.94751800000000008</v>
-      </c>
-      <c r="I46" s="10">
-        <f>AVERAGE(I51:I60)</f>
-        <v>22.315552500000003</v>
-      </c>
-      <c r="K46" s="9">
-        <f>AVERAGE(K51:K60)</f>
-        <v>0.51236274999999998</v>
-      </c>
-      <c r="L46" s="10">
-        <f>AVERAGE(L51:L60)</f>
-        <v>22.345009999999998</v>
-      </c>
-      <c r="N46" s="9">
-        <f>AVERAGE(N51:N60)</f>
-        <v>0.218414</v>
-      </c>
-      <c r="O46" s="10">
-        <f>AVERAGE(O51:O60)</f>
-        <v>22.387239999999998</v>
-      </c>
-      <c r="Q46" s="9">
-        <f>AVERAGE(Q51:Q60)</f>
-        <v>-3.745E-4</v>
-      </c>
-      <c r="R46" s="10">
-        <f>AVERAGE(R51:R60)</f>
-        <v>22.335697499999998</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="H47" s="9">
-        <f>STDEV(H51:H60)</f>
-        <v>3.4982567087048835E-4</v>
-      </c>
-      <c r="I47" s="10">
-        <f>STDEV(I51:I60)</f>
-        <v>3.1823759860624558E-2</v>
-      </c>
-      <c r="K47" s="9">
-        <f>STDEV(K51:K60)</f>
-        <v>4.0161704396105946E-4</v>
-      </c>
-      <c r="L47" s="10">
-        <f>STDEV(L51:L60)</f>
-        <v>2.3824492999153329E-2</v>
-      </c>
-      <c r="N47" s="9">
-        <f>STDEV(N51:N60)</f>
-        <v>6.4849106907240769E-4</v>
-      </c>
-      <c r="O47" s="10">
-        <f>STDEV(O51:O60)</f>
-        <v>3.0061910562481638E-2</v>
-      </c>
-      <c r="Q47" s="9">
-        <f>STDEV(Q51:Q60)</f>
-        <v>8.0289061106313453E-5</v>
-      </c>
-      <c r="R47" s="10">
-        <f>STDEV(R51:R60)</f>
-        <v>3.0177420228817243E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="H48" s="11">
-        <f>H47/H46</f>
-        <v>3.6920213744803614E-4</v>
-      </c>
-      <c r="I48" s="11">
-        <f>I47/I46</f>
-        <v>1.4260798544254978E-3</v>
-      </c>
-      <c r="K48" s="11">
-        <f>K47/K46</f>
-        <v>7.8385293224587363E-4</v>
-      </c>
-      <c r="L48" s="11">
-        <f>L47/L46</f>
-        <v>1.0662108899997507E-3</v>
-      </c>
-      <c r="N48" s="11">
-        <f>N47/N46</f>
-        <v>2.9690911254425436E-3</v>
-      </c>
-      <c r="O48" s="11">
-        <f>O47/O46</f>
-        <v>1.3428145033725302E-3</v>
-      </c>
-      <c r="Q48" s="11">
-        <f>Q47/Q46</f>
-        <v>-0.21439001630524288</v>
-      </c>
-      <c r="R48" s="11">
-        <f>R47/R46</f>
-        <v>1.3510847480280052E-3</v>
-      </c>
-    </row>
-    <row r="49" spans="8:18" x14ac:dyDescent="0.15">
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="K49" s="11"/>
-      <c r="L49" s="11"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-    </row>
-    <row r="51" spans="8:18" x14ac:dyDescent="0.15">
-      <c r="H51" s="7">
-        <v>0.94756799999999997</v>
-      </c>
-      <c r="I51" s="7">
-        <v>22.326419999999999</v>
-      </c>
-      <c r="K51" s="7">
-        <v>0.51254699999999997</v>
-      </c>
-      <c r="L51" s="7">
-        <v>22.310269999999999</v>
-      </c>
-      <c r="N51" s="7">
-        <v>0.21909000000000001</v>
-      </c>
-      <c r="O51" s="7">
-        <v>22.408359999999998</v>
-      </c>
-      <c r="Q51" s="7">
-        <v>-3.59E-4</v>
-      </c>
-      <c r="R51" s="7">
-        <v>22.351199999999999</v>
-      </c>
-    </row>
-    <row r="52" spans="8:18" x14ac:dyDescent="0.15">
-      <c r="H52" s="7">
-        <v>0.94742999999999999</v>
-      </c>
-      <c r="I52" s="7">
-        <v>22.268129999999999</v>
-      </c>
-      <c r="K52" s="7">
-        <v>0.51281100000000002</v>
-      </c>
-      <c r="L52" s="7">
-        <v>22.34995</v>
-      </c>
-      <c r="N52" s="7">
-        <v>0.217916</v>
-      </c>
-      <c r="O52" s="7">
-        <v>22.34995</v>
-      </c>
-      <c r="Q52" s="7">
-        <v>-4.17E-4</v>
-      </c>
-      <c r="R52" s="7">
-        <v>22.34995</v>
-      </c>
-    </row>
-    <row r="53" spans="8:18" x14ac:dyDescent="0.15">
-      <c r="H53" s="7">
-        <v>0.947959</v>
-      </c>
-      <c r="I53" s="7">
-        <v>22.33258</v>
-      </c>
-      <c r="K53" s="7">
-        <v>0.51188999999999996</v>
-      </c>
-      <c r="L53" s="7">
-        <v>22.356200000000001</v>
-      </c>
-      <c r="N53" s="7">
-        <v>0.217805</v>
-      </c>
-      <c r="O53" s="7">
-        <v>22.41461</v>
-      </c>
-      <c r="Q53" s="7">
-        <v>-4.5300000000000001E-4</v>
-      </c>
-      <c r="R53" s="7">
-        <v>22.351199999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="8:18" x14ac:dyDescent="0.15">
-      <c r="H54" s="7">
-        <v>0.94711500000000004</v>
-      </c>
-      <c r="I54" s="7">
-        <v>22.335080000000001</v>
-      </c>
-      <c r="K54" s="7">
-        <v>0.51220299999999996</v>
-      </c>
-      <c r="L54" s="7">
-        <v>22.363620000000001</v>
-      </c>
-      <c r="N54" s="7">
-        <v>0.21884500000000001</v>
-      </c>
-      <c r="O54" s="7">
-        <v>22.37604</v>
-      </c>
-      <c r="Q54" s="7">
-        <v>-2.6899999999999998E-4</v>
-      </c>
-      <c r="R54" s="7">
-        <v>22.29044</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>